<commit_message>
a lil more weight
</commit_message>
<xml_diff>
--- a/changes/aug-stuff.xlsx
+++ b/changes/aug-stuff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A7F395-6640-4FDF-A002-40471FB850AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A26AD6-A2F7-4B0E-8189-E7A5035EC140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1107,7 +1107,7 @@
   <dimension ref="A1:AC34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,7 +1326,7 @@
         <v>2</v>
       </c>
       <c r="Q5">
-        <v>0.59</v>
+        <v>0.6</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="AA5">
         <f t="shared" si="1"/>
-        <v>-7.3999999999999986</v>
+        <v>-7.6</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -1798,10 +1798,10 @@
         <v>0</v>
       </c>
       <c r="P18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q18">
-        <v>0.23</v>
+        <v>0.26</v>
       </c>
       <c r="R18">
         <v>0</v>
@@ -1814,11 +1814,11 @@
       </c>
       <c r="AA18">
         <f t="shared" si="1"/>
-        <v>-3.0000000000000004</v>
+        <v>-2.6</v>
       </c>
       <c r="AC18">
         <f t="shared" si="2"/>
-        <v>-0.60000000000000053</v>
+        <v>-0.20000000000000018</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
@@ -1833,10 +1833,10 @@
         <v>0</v>
       </c>
       <c r="P19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q19">
-        <v>0.23</v>
+        <v>0.26</v>
       </c>
       <c r="R19">
         <v>0</v>
@@ -1849,11 +1849,11 @@
       </c>
       <c r="AA19">
         <f t="shared" si="1"/>
-        <v>-3.0000000000000004</v>
+        <v>-2.6</v>
       </c>
       <c r="AC19">
         <f t="shared" si="2"/>
-        <v>-0.60000000000000053</v>
+        <v>-0.20000000000000018</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add new aug top rails
</commit_message>
<xml_diff>
--- a/changes/aug-stuff.xlsx
+++ b/changes/aug-stuff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A26AD6-A2F7-4B0E-8189-E7A5035EC140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53AFF23-55C3-4E02-955C-87FCD93F71EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
   <si>
     <t>old</t>
   </si>
@@ -264,6 +264,36 @@
   </si>
   <si>
     <t>AUG A3SF Top Rail 2</t>
+  </si>
+  <si>
+    <t>Steyr AUG-Z Subcompact SWAT Keymod Top Rail</t>
+  </si>
+  <si>
+    <t>steyr_aug_z_subcompact_swat_keymod_top_rail</t>
+  </si>
+  <si>
+    <t>steyr_aug_z_rail_front_sight</t>
+  </si>
+  <si>
+    <t>steyr_aug_z_rail_front_sight_folded</t>
+  </si>
+  <si>
+    <t>steyr_aug_z_rail_rear_sight</t>
+  </si>
+  <si>
+    <t>steyr_aug_z_rail_rear_sight_folded</t>
+  </si>
+  <si>
+    <t>Steyr AUG-Z Rail Front Sight</t>
+  </si>
+  <si>
+    <t>Steyr AUG-Z Rail Front Sight Folded</t>
+  </si>
+  <si>
+    <t>Steyr AUG-Z Rail Rear Sight Folded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steyr AUG-Z Rail Rear Sight </t>
   </si>
 </sst>
 </file>
@@ -1104,16 +1134,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC34"/>
+  <dimension ref="A1:AC40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -1227,7 +1257,7 @@
         <v>1000</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N34" si="0">C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*5+J3/300</f>
+        <f t="shared" ref="N3:N40" si="0">C3-D3*20-E3*0.8-F3*0.6-H3*5+I3*5+J3/300</f>
         <v>-5.0000000000000009</v>
       </c>
       <c r="P3">
@@ -1246,7 +1276,7 @@
         <v>1000</v>
       </c>
       <c r="AA3">
-        <f t="shared" ref="AA3:AA34" si="1">P3-Q3*20-R3*0.8-S3*0.6-U3*5+V3*5+W3/300</f>
+        <f t="shared" ref="AA3:AA40" si="1">P3-Q3*20-R3*0.8-S3*0.6-U3*5+V3*5+W3/300</f>
         <v>-5.0000000000000009</v>
       </c>
     </row>
@@ -1326,7 +1356,7 @@
         <v>2</v>
       </c>
       <c r="Q5">
-        <v>0.6</v>
+        <v>0.64</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -1339,7 +1369,7 @@
       </c>
       <c r="AA5">
         <f t="shared" si="1"/>
-        <v>-7.6</v>
+        <v>-8.4</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
@@ -1474,7 +1504,7 @@
         <v>5</v>
       </c>
       <c r="Q9">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="R9">
         <v>1</v>
@@ -1487,7 +1517,7 @@
       </c>
       <c r="AA9">
         <f t="shared" si="1"/>
-        <v>0.60000000000000009</v>
+        <v>0.39999999999999991</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
@@ -1520,313 +1550,305 @@
         <v>2</v>
       </c>
       <c r="Q10">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="R10">
         <v>-1</v>
       </c>
       <c r="S10">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="Z10">
         <v>750</v>
       </c>
       <c r="AA10">
         <f t="shared" si="1"/>
-        <v>0.19999999999999984</v>
+        <v>0.59999999999999964</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="N11">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>0.16</v>
+      </c>
+      <c r="R11">
+        <v>-3</v>
+      </c>
+      <c r="S11">
+        <v>-1</v>
+      </c>
+      <c r="Z11">
+        <v>1200</v>
       </c>
       <c r="AA11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.80000000000000016</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12">
-        <v>-4</v>
-      </c>
-      <c r="D12">
-        <v>0.13</v>
-      </c>
-      <c r="E12">
-        <v>-1</v>
-      </c>
-      <c r="M12">
-        <v>400</v>
-      </c>
       <c r="N12">
         <f t="shared" si="0"/>
-        <v>-5.8</v>
-      </c>
-      <c r="P12">
-        <v>-2</v>
-      </c>
-      <c r="Q12">
-        <v>0.1</v>
-      </c>
-      <c r="R12">
-        <v>-1</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="Z12">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="AA12">
         <f t="shared" si="1"/>
-        <v>-3.2</v>
-      </c>
-      <c r="AC12">
-        <f>AA12+2.4</f>
-        <v>-0.80000000000000027</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="C13">
+        <v>-4</v>
+      </c>
+      <c r="D13">
+        <v>0.13</v>
+      </c>
+      <c r="E13">
+        <v>-1</v>
+      </c>
+      <c r="M13">
+        <v>400</v>
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-5.8</v>
       </c>
       <c r="P13">
         <v>-2</v>
       </c>
       <c r="Q13">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="R13">
         <v>-1</v>
       </c>
       <c r="S13">
-        <v>-2</v>
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>400</v>
       </c>
       <c r="AA13">
         <f t="shared" si="1"/>
-        <v>-2.5999999999999996</v>
+        <v>-3.2</v>
       </c>
       <c r="AC13">
-        <f t="shared" ref="AC13:AC19" si="2">AA13+2.4</f>
-        <v>-0.19999999999999973</v>
+        <f>AA13+2.4</f>
+        <v>-0.80000000000000027</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>-2</v>
+      </c>
+      <c r="Q14">
+        <v>0.13</v>
+      </c>
+      <c r="R14">
+        <v>-1</v>
+      </c>
+      <c r="S14">
+        <v>-2</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="1"/>
+        <v>-2.5999999999999996</v>
+      </c>
+      <c r="AC14">
+        <f t="shared" ref="AC14:AC20" si="2">AA14+2.4</f>
+        <v>-0.19999999999999973</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>55</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>-5</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>0.17</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
         <v>-3</v>
       </c>
-      <c r="M14">
+      <c r="M15">
         <v>600</v>
       </c>
-      <c r="N14">
+      <c r="N15">
         <f t="shared" si="0"/>
         <v>-6.6000000000000005</v>
       </c>
-      <c r="P14">
+      <c r="P15">
         <v>1</v>
       </c>
-      <c r="Q14">
+      <c r="Q15">
         <v>0.17</v>
       </c>
-      <c r="R14">
-        <v>-1</v>
-      </c>
-      <c r="S14">
+      <c r="R15">
+        <v>-1</v>
+      </c>
+      <c r="S15">
         <v>-3</v>
       </c>
-      <c r="Z14">
+      <c r="Z15">
         <v>600</v>
       </c>
-      <c r="AA14">
+      <c r="AA15">
         <f t="shared" si="1"/>
         <v>0.19999999999999951</v>
       </c>
-      <c r="AC14">
+      <c r="AC15">
         <f t="shared" si="2"/>
         <v>2.5999999999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>57</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>58</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>-2</v>
       </c>
-      <c r="D15">
+      <c r="D16">
         <v>0.15</v>
       </c>
-      <c r="E15">
-        <v>-1</v>
-      </c>
-      <c r="M15">
+      <c r="E16">
+        <v>-1</v>
+      </c>
+      <c r="M16">
         <v>800</v>
       </c>
-      <c r="N15">
+      <c r="N16">
         <f t="shared" si="0"/>
         <v>-4.2</v>
       </c>
-      <c r="P15">
+      <c r="P16">
         <v>-3</v>
       </c>
-      <c r="Q15">
+      <c r="Q16">
         <v>0.15</v>
       </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>-1</v>
-      </c>
-      <c r="Z15">
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>-1</v>
+      </c>
+      <c r="Z16">
         <v>800</v>
       </c>
-      <c r="AA15">
+      <c r="AA16">
         <f t="shared" si="1"/>
         <v>-5.4</v>
       </c>
-      <c r="AC15">
+      <c r="AC16">
         <f t="shared" si="2"/>
         <v>-3.0000000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>59</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>60</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>-5</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>0.15</v>
       </c>
-      <c r="E16">
-        <v>-1</v>
-      </c>
-      <c r="M16">
+      <c r="E17">
+        <v>-1</v>
+      </c>
+      <c r="M17">
         <v>750</v>
       </c>
-      <c r="N16">
+      <c r="N17">
         <f t="shared" si="0"/>
         <v>-7.2</v>
       </c>
-      <c r="P16">
-        <v>-1</v>
-      </c>
-      <c r="Q16">
+      <c r="P17">
+        <v>-1</v>
+      </c>
+      <c r="Q17">
         <v>0.14000000000000001</v>
       </c>
-      <c r="R16">
-        <v>-1</v>
-      </c>
-      <c r="S16">
-        <v>-1</v>
-      </c>
-      <c r="Z16">
+      <c r="R17">
+        <v>-1</v>
+      </c>
+      <c r="S17">
+        <v>-1</v>
+      </c>
+      <c r="Z17">
         <v>750</v>
       </c>
-      <c r="AA16">
+      <c r="AA17">
         <f t="shared" si="1"/>
         <v>-2.4</v>
-      </c>
-      <c r="AC16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="N17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Z17">
-        <v>800</v>
-      </c>
-      <c r="AA17">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
       <c r="AC17">
         <f t="shared" si="2"/>
-        <v>2.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" t="s">
-        <v>62</v>
-      </c>
       <c r="N18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P18">
-        <v>2</v>
-      </c>
-      <c r="Q18">
-        <v>0.26</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>-1</v>
-      </c>
       <c r="Z18">
-        <v>3000</v>
+        <v>800</v>
       </c>
       <c r="AA18">
         <f t="shared" si="1"/>
-        <v>-2.6</v>
+        <v>0</v>
       </c>
       <c r="AC18">
         <f t="shared" si="2"/>
-        <v>-0.20000000000000018</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N19">
         <f t="shared" si="0"/>
@@ -1845,7 +1867,7 @@
         <v>-1</v>
       </c>
       <c r="Z19">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="AA19">
         <f t="shared" si="1"/>
@@ -1857,333 +1879,349 @@
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
       <c r="N20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>0.26</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>-1</v>
+      </c>
+      <c r="Z20">
+        <v>2000</v>
+      </c>
       <c r="AA20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2.6</v>
+      </c>
+      <c r="AC20">
+        <f t="shared" si="2"/>
+        <v>-0.20000000000000018</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>65</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>66</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>2</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <v>0.16</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
         <v>-5</v>
       </c>
-      <c r="M21">
+      <c r="M22">
         <v>800</v>
       </c>
-      <c r="N21">
+      <c r="N22">
         <f t="shared" si="0"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="P21">
+      <c r="P22">
         <v>2</v>
       </c>
-      <c r="Q21">
+      <c r="Q22">
         <v>0.11</v>
       </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
         <v>-4</v>
       </c>
-      <c r="Z21">
+      <c r="Z22">
         <v>800</v>
       </c>
-      <c r="AA21">
+      <c r="AA22">
         <f t="shared" si="1"/>
         <v>2.1999999999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="N22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
-      </c>
-      <c r="D23">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E23">
-        <v>-2</v>
-      </c>
-      <c r="F23">
-        <v>-2</v>
-      </c>
-      <c r="M23">
-        <v>800</v>
-      </c>
       <c r="N23">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="P23">
-        <v>3</v>
-      </c>
-      <c r="Q23">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="R23">
-        <v>-2</v>
-      </c>
-      <c r="S23">
-        <v>-2</v>
-      </c>
-      <c r="Z23">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="AA23">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C24">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="D24">
-        <v>0.06</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E24">
         <v>-2</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="N24">
         <f t="shared" si="0"/>
-        <v>-0.60000000000000009</v>
+        <v>3</v>
       </c>
       <c r="P24">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Q24">
-        <v>0.06</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="R24">
         <v>-2</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Z24">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="AA24">
         <f t="shared" si="1"/>
-        <v>-0.60000000000000009</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25">
+        <v>-1</v>
+      </c>
+      <c r="D25">
+        <v>0.06</v>
+      </c>
+      <c r="E25">
+        <v>-2</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>-0.60000000000000009</v>
+      </c>
+      <c r="P25">
+        <v>-1</v>
+      </c>
+      <c r="Q25">
+        <v>0.06</v>
+      </c>
+      <c r="R25">
+        <v>-2</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="1"/>
+        <v>-0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>38</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>-0.5</v>
       </c>
-      <c r="D25">
+      <c r="D26">
         <v>0.04</v>
       </c>
-      <c r="E25">
-        <v>-1</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25">
+      <c r="E26">
+        <v>-1</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
         <f t="shared" si="0"/>
         <v>-0.5</v>
       </c>
-      <c r="P25">
+      <c r="P26">
         <v>-0.5</v>
       </c>
-      <c r="Q25">
+      <c r="Q26">
         <v>0.04</v>
       </c>
-      <c r="R25">
-        <v>-1</v>
-      </c>
-      <c r="S25">
-        <v>0</v>
-      </c>
-      <c r="Z25">
-        <v>0</v>
-      </c>
-      <c r="AA25">
+      <c r="R26">
+        <v>-1</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
         <f t="shared" si="1"/>
         <v>-0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="N26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>1000</v>
-      </c>
       <c r="N27">
         <f t="shared" si="0"/>
-        <v>-1.4000000000000001</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
-      <c r="Z27">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AA27">
         <f t="shared" si="1"/>
-        <v>-1.4000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>1000</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>-1.4000000000000001</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>1000</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="1"/>
+        <v>-1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>42</v>
       </c>
-      <c r="C28">
-        <v>-1</v>
-      </c>
-      <c r="D28">
+      <c r="C29">
+        <v>-1</v>
+      </c>
+      <c r="D29">
         <v>0.06</v>
       </c>
-      <c r="E28">
-        <v>-1</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="M28">
+      <c r="E29">
+        <v>-1</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="M29">
         <v>1200</v>
       </c>
-      <c r="N28">
+      <c r="N29">
         <f t="shared" si="0"/>
         <v>-1.4000000000000001</v>
       </c>
-      <c r="P28">
-        <v>-1</v>
-      </c>
-      <c r="Q28">
+      <c r="P29">
+        <v>-1</v>
+      </c>
+      <c r="Q29">
         <v>0.06</v>
       </c>
-      <c r="R28">
-        <v>-1</v>
-      </c>
-      <c r="S28">
-        <v>0</v>
-      </c>
-      <c r="Z28">
+      <c r="R29">
+        <v>-1</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="Z29">
         <v>1200</v>
       </c>
-      <c r="AA28">
+      <c r="AA29">
         <f t="shared" si="1"/>
         <v>-1.4000000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="N29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" t="s">
-        <v>68</v>
-      </c>
       <c r="N30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Z30">
         <v>0</v>
       </c>
       <c r="AA30">
@@ -2193,10 +2231,10 @@
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N31">
         <f t="shared" si="0"/>
@@ -2212,10 +2250,10 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N32">
         <f t="shared" si="0"/>
@@ -2231,10 +2269,10 @@
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N33">
         <f t="shared" si="0"/>
@@ -2250,21 +2288,150 @@
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>75</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>76</v>
       </c>
-      <c r="N34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Z34">
-        <v>0</v>
-      </c>
-      <c r="AA34">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="N35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z35">
+        <v>0</v>
+      </c>
+      <c r="AA35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" t="s">
+        <v>83</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>3</v>
+      </c>
+      <c r="Q37">
+        <v>0.03</v>
+      </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
+      <c r="AA37">
+        <f t="shared" si="1"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>2</v>
+      </c>
+      <c r="Q38">
+        <v>0.03</v>
+      </c>
+      <c r="Z38">
+        <v>0</v>
+      </c>
+      <c r="AA38">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" t="s">
+        <v>86</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>3</v>
+      </c>
+      <c r="Q39">
+        <v>0.03</v>
+      </c>
+      <c r="Z39">
+        <v>0</v>
+      </c>
+      <c r="AA39">
+        <f t="shared" si="1"/>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>2</v>
+      </c>
+      <c r="Q40">
+        <v>0.03</v>
+      </c>
+      <c r="Z40">
+        <v>0</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>